<commit_message>
cmd/roi: 엑셀 파일에 thumbnail 컬럼 추가
웹에서 엑셀 업로드시 썸네일을 함께 전송하는 것을 테스트하기
위한 데이터 추가.
</commit_message>
<xml_diff>
--- a/cmd/roi/testdata/test.xlsx
+++ b/cmd/roi/testdata/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
   <si>
     <t xml:space="preserve">show</t>
   </si>
@@ -51,6 +51,9 @@
     <t xml:space="preserve">duration</t>
   </si>
   <si>
+    <t xml:space="preserve">thumbnail</t>
+  </si>
+  <si>
     <t xml:space="preserve">tags</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve">00:08:15:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/vfx/thumbnail1.jpg</t>
   </si>
   <si>
     <r>
@@ -84,6 +90,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">로이</t>
     </r>
@@ -103,6 +110,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">가나다라마바사아자차카타파하</t>
     </r>
@@ -122,6 +130,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">고노도로모보소호조초코토포호</t>
     </r>
@@ -136,6 +145,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">조용한 카페에 앉아 길을 지나가는 사람들의 표정을 살핀다</t>
     </r>
@@ -157,6 +167,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">배경 리플레이스</t>
     </r>
@@ -176,6 +187,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">휘핑크림 추가</t>
     </r>
@@ -185,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">00:02:01:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/vfx/thumbnail2.jpg</t>
   </si>
   <si>
     <r>
@@ -193,6 +208,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">로이</t>
     </r>
@@ -212,6 +228,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">카페</t>
     </r>
@@ -231,6 +248,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">휘핑크림</t>
     </r>
@@ -254,6 +272,9 @@
     <t xml:space="preserve">00:01:10:12</t>
   </si>
   <si>
+    <t xml:space="preserve">/vfx/thumbnail3.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">로이</t>
   </si>
   <si>
@@ -272,6 +293,9 @@
     <t xml:space="preserve">00:02:37:15</t>
   </si>
   <si>
+    <t xml:space="preserve">/vfx/thumbnail4.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">0050</t>
   </si>
   <si>
@@ -285,6 +309,9 @@
   </si>
   <si>
     <t xml:space="preserve">17:22:39:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/vfx/thumbnail5.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">북두칠성</t>
@@ -302,6 +329,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">책 제목 수정 </t>
     </r>
@@ -321,6 +349,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">북두칠성</t>
     </r>
@@ -342,6 +371,9 @@
     <t xml:space="preserve">00:24:32:00</t>
   </si>
   <si>
+    <t xml:space="preserve">/vfx/thumbnail6.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">0070</t>
   </si>
   <si>
@@ -355,6 +387,9 @@
   </si>
   <si>
     <t xml:space="preserve">00:27:41:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/vfx/thumbnail7.jpg</t>
   </si>
   <si>
     <r>
@@ -363,6 +398,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">로이</t>
     </r>
@@ -382,6 +418,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">공원</t>
     </r>
@@ -405,6 +442,9 @@
     <t xml:space="preserve">17:21:40:10</t>
   </si>
   <si>
+    <t xml:space="preserve">/vfx/thumbnail8.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">0090</t>
   </si>
   <si>
@@ -420,6 +460,9 @@
     <t xml:space="preserve">17:29:12:19</t>
   </si>
   <si>
+    <t xml:space="preserve">/vfx/thumbnail9.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">가로등</t>
   </si>
   <si>
@@ -433,6 +476,9 @@
   </si>
   <si>
     <t xml:space="preserve">17:29:21:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/vfx/thumbnail10.jpg</t>
   </si>
 </sst>
 </file>
@@ -443,7 +489,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -471,6 +517,15 @@
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -515,7 +570,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -536,6 +591,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,13 +612,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.63671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.63671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
@@ -567,8 +626,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="11" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="12" style="0" width="7.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -602,343 +663,380 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>2073</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>205</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>24</v>
+      <c r="J3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I4" s="4" t="n">
         <v>363</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>31</v>
+      <c r="J4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I5" s="4" t="n">
         <v>1546</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>31</v>
+      <c r="J5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="I6" s="4" t="n">
         <v>2232</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>42</v>
+      <c r="J6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I7" s="4" t="n">
         <v>92</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>31</v>
+      <c r="J7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I8" s="4" t="n">
         <v>101</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>53</v>
+      <c r="J8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="I9" s="4" t="n">
         <v>72</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>140</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>65</v>
+      <c r="J10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I11" s="4" t="n">
         <v>103</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>42</v>
+      <c r="J11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>